<commit_message>
Simulador Investimento versão Final
Versão final simulador de Investimentos
</commit_message>
<xml_diff>
--- a/ferramentaDeInvestimento.xlsx
+++ b/ferramentaDeInvestimento.xlsx
@@ -1,32 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28821fe6167af94f/Área de Trabalho/Wagner Andrade/DIO/Excel/Desafio01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="691" documentId="8_{A617BF44-FAD2-4711-8CA2-2A0868C800F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B486DA77-B1B6-401C-8FBD-393153ECD032}"/>
+  <xr:revisionPtr revIDLastSave="851" documentId="8_{A617BF44-FAD2-4711-8CA2-2A0868C800F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{106F45E2-7CF3-4A0B-8F13-CE74DA9870AB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" xr2:uid="{B26E8035-E0E8-49CC-AD17-96080EA24C4E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Simulador de Investimento" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Instruções" sheetId="4" r:id="rId1"/>
+    <sheet name="Simulador de Investimento" sheetId="1" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="aporte">'Simulador de Investimento'!$D$16</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Simulador de Investimento'!$A$1:$E$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Instruções!$A$1:$L$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Simulador de Investimento'!$A$1:$E$60</definedName>
     <definedName name="patrimonio">'Simulador de Investimento'!$D$19</definedName>
     <definedName name="qtd_anos">'Simulador de Investimento'!$D$17</definedName>
     <definedName name="rendimento_carteira">'Simulador de Investimento'!$D$12</definedName>
     <definedName name="salario">'Simulador de Investimento'!$D$11</definedName>
     <definedName name="sugestao_investimento">'Simulador de Investimento'!$D$13</definedName>
     <definedName name="taxa_mensal">'Simulador de Investimento'!$D$18</definedName>
-    <definedName name="Z_4DED35F6_E813_4E51_8B55_7DA6C214AEF7_.wvu.Cols" localSheetId="0" hidden="1">'Simulador de Investimento'!$F:$XFD</definedName>
-    <definedName name="Z_4DED35F6_E813_4E51_8B55_7DA6C214AEF7_.wvu.PrintArea" localSheetId="0" hidden="1">'Simulador de Investimento'!$A$1:$E$55</definedName>
+    <definedName name="Z_4DED35F6_E813_4E51_8B55_7DA6C214AEF7_.wvu.Cols" localSheetId="1" hidden="1">'Simulador de Investimento'!$F:$XFD</definedName>
+    <definedName name="Z_4DED35F6_E813_4E51_8B55_7DA6C214AEF7_.wvu.PrintArea" localSheetId="1" hidden="1">'Simulador de Investimento'!$A$1:$E$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t>Quanto tempo investir</t>
   </si>
@@ -157,6 +159,13 @@
   </si>
   <si>
     <t>Acumulado</t>
+  </si>
+  <si>
+    <t>Como parte do primeiro desafio do Curso Santander - Excel com Inteligência Artificial da DIO, criei um simulador de investimentos em Excel que oferece uma ferramenta simples para planejamento financeiro pessoal.
+Este simulador guia o usuário por um fluxo intuitivo, começando pelo painel de Configurações, onde o salário e o rendimento da carteira são informados. Com base nesses dados, o sistema calcula e exibe o valor ideal a ser investido, servindo como um ponto de partida estratégico.
+A funcionalidade central reside no painel Investimento Inicial, onde o usuário pode projetar cenários inserindo o montante a ser investido, o horizonte de tempo (em anos) e a taxa de rendimento mensal. Instantaneamente, o simulador retorna o Patrimônio Acumulado e os Dividendos esperados ao final do prazo.
+Para uma visão abrangente do futuro, o painel Cenários oferece projeções automáticas de valores acumulados e dividendos para horizontes de 2, 5, 10, 20 e 30 anos, permitindo uma análise comparativa eficaz.
+Por fim, a ferramenta se aprofunda no planejamento prático através de um simulador de investimento mensal, que sugere a distribuição de aportes de acordo com o perfil de investidor (Conservador, Moderado ou Agressivo). Essa orientação é visualizada de forma clara por meio de um gráfico de pizza, otimizando a alocação de recursos.</t>
   </si>
 </sst>
 </file>
@@ -629,7 +638,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -679,21 +688,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="12" fillId="7" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -701,9 +695,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="7" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -711,26 +702,11 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="165" fontId="12" fillId="7" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -740,47 +716,87 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="8" fontId="5" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Entrada" xfId="4" builtinId="20"/>
@@ -1880,6 +1896,205 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1380565</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo: Cantos Arredondados 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2989468C-9288-4A4B-884D-6A195BE25B2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="259976" y="38100"/>
+          <a:ext cx="7153836" cy="1378324"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:effectLst>
+          <a:innerShdw blurRad="114300">
+            <a:prstClr val="black"/>
+          </a:innerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textCascadeUp">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 38111"/>
+            </a:avLst>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Simulador de Investimentos</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0">
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100">
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2554042</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>26890</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1667434</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>17925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Retângulo: Cantos Arredondados 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95EFAB40-3E08-1843-2D80-99D45CEBA8AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2814018" y="6122890"/>
+          <a:ext cx="2044851" cy="349623"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Simulador de Investimentos</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1916,7 +2131,7 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
@@ -2027,6 +2242,84 @@
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2339340</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1449594</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>82923</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Retângulo: Cantos Arredondados 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78C0B382-FBB8-4CD4-B561-5C5C390572B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2598420" y="11513820"/>
+          <a:ext cx="2043954" cy="349623"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Instruções</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2355,13 +2648,383 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7150C880-5218-4750-9F37-3F2AB4E95E91}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M51"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D33"/>
+      <extLst>
+        <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
+          <xlsdti:showDataTypeIcons visible="0"/>
+        </ext>
+      </extLst>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="2" max="2" width="42.77734375" customWidth="1"/>
+    <col min="3" max="3" width="41.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="3.77734375" customWidth="1"/>
+    <col min="6" max="11" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="3.77734375" hidden="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+    </row>
+    <row r="11" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+    </row>
+    <row r="12" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+    </row>
+    <row r="13" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+    </row>
+    <row r="14" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+    </row>
+    <row r="15" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+    </row>
+    <row r="16" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+    </row>
+    <row r="17" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+    </row>
+    <row r="18" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+    </row>
+    <row r="19" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+    </row>
+    <row r="20" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+    </row>
+    <row r="21" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+    </row>
+    <row r="22" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+    </row>
+    <row r="23" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+    </row>
+    <row r="24" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+    </row>
+    <row r="25" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+    </row>
+    <row r="26" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+    </row>
+    <row r="27" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
+    </row>
+    <row r="28" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+    </row>
+    <row r="29" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+    </row>
+    <row r="30" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+    </row>
+    <row r="31" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+    </row>
+    <row r="32" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+    </row>
+    <row r="33" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3"/>
+    <row r="49" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="50" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="51" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="B10:D33"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup scale="95" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DAA491-A54D-4411-89F8-E67D237E8C49}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" view="pageBreakPreview" topLeftCell="A29" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
@@ -2390,104 +3053,104 @@
     <row r="8" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:4" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
     </row>
     <row r="11" spans="2:4" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29">
+      <c r="C11" s="45"/>
+      <c r="D11" s="24">
         <v>1000</v>
       </c>
     </row>
     <row r="12" spans="2:4" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32">
+      <c r="C12" s="47"/>
+      <c r="D12" s="26">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="2:4" s="2" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35">
+      <c r="C13" s="49"/>
+      <c r="D13" s="28">
         <f>D11*30%</f>
         <v>300</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="43"/>
     </row>
     <row r="16" spans="2:4" s="2" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41">
+      <c r="C16" s="54"/>
+      <c r="D16" s="30">
         <v>300</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="42">
+      <c r="C17" s="54"/>
+      <c r="D17" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="32">
+      <c r="C18" s="54"/>
+      <c r="D18" s="26">
         <v>1.0789999999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="2" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45">
+      <c r="C19" s="56"/>
+      <c r="D19" s="32">
         <f>FV(taxa_mensal,(qtd_anos*12),(aporte*-1))</f>
         <v>25133.074199546292</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="2" customFormat="1" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48">
+      <c r="C20" s="58"/>
+      <c r="D20" s="33">
         <f>patrimonio*rendimento_carteira</f>
         <v>150.79844519727774</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:4" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="51" t="s">
+      <c r="D22" s="35" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2495,14 +3158,14 @@
       <c r="A23" s="3">
         <v>2</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="53">
+      <c r="C23" s="36">
         <f>FV($D$18,($A23*12),(-$D$16))</f>
         <v>8168.2881892935648</v>
       </c>
-      <c r="D23" s="54">
+      <c r="D23" s="37">
         <f>C23*rendimento_carteira</f>
         <v>49.00972913576139</v>
       </c>
@@ -2511,14 +3174,14 @@
       <c r="A24" s="3">
         <v>5</v>
       </c>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="53">
+      <c r="C24" s="36">
         <f>FV($D$18,($A24*12),(-$D$16))</f>
         <v>25133.074199546292</v>
       </c>
-      <c r="D24" s="54">
+      <c r="D24" s="37">
         <f>C24*rendimento_carteira</f>
         <v>150.79844519727774</v>
       </c>
@@ -2527,14 +3190,14 @@
       <c r="A25" s="3">
         <v>10</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="53">
+      <c r="C25" s="36">
         <f>FV($D$18,($A25*12),(-$D$16))</f>
         <v>72985.263759051653</v>
       </c>
-      <c r="D25" s="54">
+      <c r="D25" s="37">
         <f>C25*rendimento_carteira</f>
         <v>437.91158255430992</v>
       </c>
@@ -2543,14 +3206,14 @@
       <c r="A26" s="3">
         <v>20</v>
       </c>
-      <c r="B26" s="52" t="s">
+      <c r="B26" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="53">
+      <c r="C26" s="36">
         <f>FV($D$18,($A26*12),(-$D$16))</f>
         <v>337559.52002912416</v>
       </c>
-      <c r="D26" s="54">
+      <c r="D26" s="37">
         <f>C26*rendimento_carteira</f>
         <v>2025.357120174745</v>
       </c>
@@ -2559,14 +3222,14 @@
       <c r="A27" s="3">
         <v>30</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="56">
+      <c r="C27" s="38">
         <f>FV($D$18,($A27*12),(-$D$16))</f>
         <v>1296650.8965014142</v>
       </c>
-      <c r="D27" s="57">
+      <c r="D27" s="39">
         <f>C27*rendimento_carteira</f>
         <v>7779.9053790084854</v>
       </c>
@@ -2698,15 +3361,22 @@
     <row r="46" spans="2:4" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:4" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
     <row r="48" spans="2:4" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="49" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="50" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="51" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="52" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="53" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="54" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="55" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="2:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="2:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="2:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="2:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="2:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="2:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B60" s="59"/>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <customSheetViews>
     <customSheetView guid="{4DED35F6-E813-4E51-8B55-7DA6C214AEF7}" scale="85" showPageBreaks="1" showGridLines="0" showRowCol="0" fitToPage="1" printArea="1" hiddenColumns="1">
       <selection activeCell="C28" sqref="C28"/>
@@ -2737,12 +3407,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="83" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="77" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18C5803-D2AB-4AFB-8780-783688478538}">
   <dimension ref="A2:D20"/>
   <sheetViews>

</xml_diff>